<commit_message>
Fix: Bổ sung điều kiện chỉ xuất cho công tác viên là nhân viên
</commit_message>
<xml_diff>
--- a/reportTemplate/report_danh_sach_ctv.xlsx
+++ b/reportTemplate/report_danh_sach_ctv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/Project/MCOM/mobifone/pshop/reportTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1C10D2-B82A-DF4E-8BE2-1DC6CC5256CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ADBE44-0D1F-EA44-B363-CF870ED73606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{2536DECE-D6AB-F14D-B214-39325C1EFF7A}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>